<commit_message>
add tests for only year det
</commit_message>
<xml_diff>
--- a/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
+++ b/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\laji.fi-front\projects\laji\e2e\src\+vihko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A650AB-E09E-426F-B17F-C38050C5E170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D9CB25-7E8C-4B00-9ACA-556A6240F55A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2505" windowWidth="24285" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="24285" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tallennuspohja" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="575">
   <si>
     <t>Muokkausoikeus - Havaintoerä</t>
   </si>
@@ -1741,6 +1741,12 @@
   </si>
   <si>
     <t>2020-3-01</t>
+  </si>
+  <si>
+    <t>Viltsu</t>
+  </si>
+  <si>
+    <t>Masa</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BD4" sqref="BD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2379,6 +2385,12 @@
       <c r="BC2" t="s">
         <v>566</v>
       </c>
+      <c r="BD2" t="s">
+        <v>573</v>
+      </c>
+      <c r="BE2">
+        <v>2020</v>
+      </c>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2419,6 +2431,12 @@
       </c>
       <c r="BC3" t="s">
         <v>568</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>574</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>44197</v>
       </c>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.25">
@@ -2463,7 +2481,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:BR1 A2:D2 I2:J2 L2:AD2 BD2:BR2 AF2:BB2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:BR1 A2:D2 I2:J2 L2:AD2 BF2:BR2 AF2:BB2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
Small tweak and add test case for file import [fixes #177379077]
</commit_message>
<xml_diff>
--- a/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
+++ b/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\laji.fi-front\projects\laji\e2e\src\+vihko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D9CB25-7E8C-4B00-9ACA-556A6240F55A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639C5936-C336-4CC3-8F03-6AF7A23B30D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="24285" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="24285" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tallennuspohja" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="576">
   <si>
     <t>Muokkausoikeus - Havaintoerä</t>
   </si>
@@ -1747,6 +1747,9 @@
   </si>
   <si>
     <t>Masa</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2131,7 @@
   <dimension ref="A1:BR4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BD4" sqref="BD4"/>
+      <selection activeCell="BF4" sqref="BF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2475,6 +2478,9 @@
       </c>
       <c r="BC4" t="s">
         <v>570</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import fails if end date not given [fixes #177488749]
</commit_message>
<xml_diff>
--- a/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
+++ b/projects/laji/e2e/src/+vihko/ValidRows(JX.519).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\laji.fi-front\projects\laji\e2e\src\+vihko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639C5936-C336-4CC3-8F03-6AF7A23B30D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF0EFB-C77C-4D70-BEA7-5202C6D27DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="24285" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="575">
   <si>
     <t>Muokkausoikeus - Havaintoerä</t>
   </si>
@@ -39,15 +39,6 @@
     <t>Alku - Yleinen keruutapahtuma</t>
   </si>
   <si>
-    <t>Loppu@dd - Yleinen keruutapahtuma</t>
-  </si>
-  <si>
-    <t>Loppu@mm - Yleinen keruutapahtuma</t>
-  </si>
-  <si>
-    <t>Loppu@yyyy - Yleinen keruutapahtuma</t>
-  </si>
-  <si>
     <t>Avainsanat - Havaintoerä</t>
   </si>
   <si>
@@ -1750,6 +1741,12 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>Loppu - Yleinen keruutapahtuma</t>
+  </si>
+  <si>
+    <t>2.3.2020</t>
   </si>
 </sst>
 </file>
@@ -2128,15 +2125,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR4"/>
+  <dimension ref="A1:BP5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BF4" sqref="BF4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2153,345 +2150,359 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>573</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43893</v>
+      </c>
+      <c r="I2" t="s">
+        <v>564</v>
+      </c>
+      <c r="AC2">
+        <v>10</v>
+      </c>
+      <c r="AH2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="AI2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+      <c r="BA2" t="s">
+        <v>563</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>570</v>
+      </c>
+      <c r="BC2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43893</v>
+      </c>
+      <c r="I3" t="s">
+        <v>564</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AH3" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>2020</v>
-      </c>
-      <c r="K2" t="s">
-        <v>567</v>
-      </c>
-      <c r="AE2">
-        <v>10</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>566</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>573</v>
-      </c>
-      <c r="BE2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AI3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>565</v>
+      </c>
+      <c r="BB3" t="s">
         <v>571</v>
       </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>2020</v>
-      </c>
-      <c r="K3" t="s">
-        <v>567</v>
-      </c>
-      <c r="AE3">
-        <v>2</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>568</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>574</v>
-      </c>
-      <c r="BE3" s="1">
+      <c r="BC3" s="1">
         <v>44197</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1">
         <v>43891</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="1">
+        <v>43893</v>
+      </c>
+      <c r="I4" t="s">
+        <v>564</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>567</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="I5" t="s">
+        <v>564</v>
+      </c>
+      <c r="AC5">
+        <v>10</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>563</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>570</v>
+      </c>
+      <c r="BC5">
         <v>2020</v>
-      </c>
-      <c r="K4" t="s">
-        <v>567</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>570</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>575</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:BR1 A2:D2 I2:J2 L2:AD2 BF2:BR2 AF2:BB2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 A2:D2 G2:H2 J2:AB2 BD2:BP2 AD2:AZ2 G1:BP1" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="26">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="24">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$A$1:$A$2</xm:f>
@@ -2502,151 +2513,139 @@
           <x14:formula1>
             <xm:f>Muuttujat!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1001 AR2:AR1001 AP2:AP1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>Muuttujat!$C$1:$C$31</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>Muuttujat!$D$1:$D$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1001</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>Muuttujat!$E$1:$E$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1001</xm:sqref>
+          <xm:sqref>AN2:AN1001 AP2:AP1001 D2:D1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$F$1:$F$87</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T1001</xm:sqref>
+          <xm:sqref>R2:R1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$G$1:$G$46</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X1001 AL2:AL1001</xm:sqref>
+          <xm:sqref>AJ2:AJ1001 V2:V1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$H$1:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD1001</xm:sqref>
+          <xm:sqref>AB2:AB1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$I$1:$I$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AH2:AH1001</xm:sqref>
+          <xm:sqref>AF2:AF1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$J$1:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AJ2:AJ1001</xm:sqref>
+          <xm:sqref>AH2:AH1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$K$1:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AK2:AK1001</xm:sqref>
+          <xm:sqref>AI2:AI1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$L$1:$L$36</xm:f>
           </x14:formula1>
-          <xm:sqref>AN2:AN1001</xm:sqref>
+          <xm:sqref>AL2:AL1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00000D000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$M$1:$M$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AO2:AO1001</xm:sqref>
+          <xm:sqref>AM2:AM1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00000F000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$N$1:$N$21</xm:f>
           </x14:formula1>
-          <xm:sqref>AQ2:AQ1001</xm:sqref>
+          <xm:sqref>AO2:AO1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$O$1:$O$13</xm:f>
           </x14:formula1>
-          <xm:sqref>AS2:AS1001</xm:sqref>
+          <xm:sqref>AQ2:AQ1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$P$1:$P$30</xm:f>
           </x14:formula1>
-          <xm:sqref>AT2:AT1001</xm:sqref>
+          <xm:sqref>AR2:AR1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000013000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$Q$1:$Q$21</xm:f>
           </x14:formula1>
-          <xm:sqref>AU2:AU1001</xm:sqref>
+          <xm:sqref>AS2:AS1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$R$1:$R$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AX2:AX1001</xm:sqref>
+          <xm:sqref>AV2:AV1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000015000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$S$1:$S$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AZ2:AZ1001</xm:sqref>
+          <xm:sqref>AX2:AX1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000016000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$T$1:$T$143</xm:f>
           </x14:formula1>
-          <xm:sqref>BB2:BB1001</xm:sqref>
+          <xm:sqref>AZ2:AZ1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000017000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$U$1:$U$12</xm:f>
           </x14:formula1>
-          <xm:sqref>BF2:BF1001</xm:sqref>
+          <xm:sqref>BD2:BD1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000018000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$V$1:$V$12</xm:f>
           </x14:formula1>
-          <xm:sqref>BJ2:BJ1001</xm:sqref>
+          <xm:sqref>BH2:BH1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000019000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$W$1:$W$19</xm:f>
           </x14:formula1>
-          <xm:sqref>BK2:BK1001</xm:sqref>
+          <xm:sqref>BI2:BI1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00001A000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$X$1:$X$5</xm:f>
           </x14:formula1>
-          <xm:sqref>BM2:BM1001</xm:sqref>
+          <xm:sqref>BK2:BK1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00001B000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$Y$1:$Y$16</xm:f>
           </x14:formula1>
-          <xm:sqref>BN2:BN1001</xm:sqref>
+          <xm:sqref>BL2:BL1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-00001C000000}">
           <x14:formula1>
             <xm:f>Muuttujat!$Z$1:$Z$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BO2:BO1001</xm:sqref>
+          <xm:sqref>BM2:BM1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" xr:uid="{068F5D83-27D3-4D03-9EA1-4D8B704EC448}">
+          <x14:formula1>
+            <xm:f>Muuttujat!$C$1:$C$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1001</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2667,7 +2666,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2688,10 +2687,10 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -2703,75 +2702,75 @@
         <v>2020</v>
       </c>
       <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>85</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>86</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>87</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>89</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>90</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>91</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>92</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>93</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>94</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>95</v>
-      </c>
-      <c r="X1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2783,67 +2782,67 @@
         <v>2019</v>
       </c>
       <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>100</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
         <v>101</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>102</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>103</v>
       </c>
-      <c r="K2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>104</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>105</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>106</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>107</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>109</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>110</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>111</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>112</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>113</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>114</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>115</v>
-      </c>
-      <c r="X2" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -2857,67 +2856,67 @@
         <v>2018</v>
       </c>
       <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" t="s">
         <v>119</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" t="s">
         <v>120</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>121</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>122</v>
       </c>
-      <c r="J3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>123</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>124</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>125</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>126</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>127</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>128</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>129</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>130</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>131</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>132</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>133</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
         <v>134</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>135</v>
-      </c>
-      <c r="X3" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -2931,61 +2930,61 @@
         <v>2017</v>
       </c>
       <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" t="s">
         <v>139</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>140</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>141</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
         <v>142</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>143</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>144</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
+        <v>84</v>
+      </c>
+      <c r="R4" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" t="s">
         <v>145</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>146</v>
       </c>
-      <c r="P4" t="s">
+      <c r="U4" t="s">
         <v>147</v>
       </c>
-      <c r="Q4" t="s">
-        <v>87</v>
-      </c>
-      <c r="R4" t="s">
-        <v>131</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>148</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>149</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>150</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Y4" t="s">
         <v>151</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>152</v>
-      </c>
-      <c r="X4" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -2999,58 +2998,58 @@
         <v>2016</v>
       </c>
       <c r="F5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
         <v>156</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>157</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>158</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
         <v>159</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" t="s">
         <v>160</v>
       </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
         <v>161</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>162</v>
       </c>
-      <c r="O5" t="s">
-        <v>118</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>163</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>164</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>165</v>
       </c>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>166</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>167</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>168</v>
       </c>
-      <c r="V5" t="s">
+      <c r="Y5" t="s">
         <v>169</v>
-      </c>
-      <c r="W5" t="s">
-        <v>170</v>
-      </c>
-      <c r="X5" t="s">
-        <v>171</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -3064,46 +3063,46 @@
         <v>2015</v>
       </c>
       <c r="F6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K6" t="s">
         <v>173</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
         <v>174</v>
       </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>175</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>176</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>177</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
+        <v>161</v>
+      </c>
+      <c r="T6" t="s">
         <v>178</v>
       </c>
-      <c r="O6" t="s">
+      <c r="U6" t="s">
         <v>179</v>
       </c>
-      <c r="P6" t="s">
+      <c r="V6" t="s">
         <v>180</v>
       </c>
-      <c r="Q6" t="s">
-        <v>164</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="W6" t="s">
         <v>181</v>
       </c>
-      <c r="U6" t="s">
+      <c r="Y6" t="s">
         <v>182</v>
-      </c>
-      <c r="V6" t="s">
-        <v>183</v>
-      </c>
-      <c r="W6" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -3117,43 +3116,43 @@
         <v>2014</v>
       </c>
       <c r="F7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="L7" t="s">
         <v>186</v>
       </c>
-      <c r="G7" t="s">
+      <c r="N7" t="s">
         <v>187</v>
       </c>
-      <c r="I7" t="s">
+      <c r="O7" t="s">
         <v>188</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>189</v>
       </c>
-      <c r="N7" t="s">
+      <c r="Q7" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" t="s">
         <v>190</v>
       </c>
-      <c r="O7" t="s">
+      <c r="U7" t="s">
         <v>191</v>
       </c>
-      <c r="P7" t="s">
+      <c r="V7" t="s">
         <v>192</v>
       </c>
-      <c r="Q7" t="s">
-        <v>107</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="W7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y7" t="s">
         <v>193</v>
-      </c>
-      <c r="U7" t="s">
-        <v>194</v>
-      </c>
-      <c r="V7" t="s">
-        <v>195</v>
-      </c>
-      <c r="W7" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -3167,43 +3166,43 @@
         <v>2013</v>
       </c>
       <c r="F8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8" t="s">
         <v>197</v>
       </c>
-      <c r="G8" t="s">
+      <c r="N8" t="s">
         <v>198</v>
       </c>
-      <c r="I8" t="s">
+      <c r="O8" t="s">
         <v>199</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" t="s">
         <v>200</v>
       </c>
-      <c r="N8" t="s">
+      <c r="Q8" t="s">
         <v>201</v>
       </c>
-      <c r="O8" t="s">
+      <c r="T8" t="s">
         <v>202</v>
       </c>
-      <c r="P8" t="s">
+      <c r="U8" t="s">
         <v>203</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="V8" t="s">
         <v>204</v>
       </c>
-      <c r="T8" t="s">
+      <c r="W8" t="s">
         <v>205</v>
       </c>
-      <c r="U8" t="s">
+      <c r="Y8" t="s">
         <v>206</v>
-      </c>
-      <c r="V8" t="s">
-        <v>207</v>
-      </c>
-      <c r="W8" t="s">
-        <v>208</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -3217,40 +3216,40 @@
         <v>2012</v>
       </c>
       <c r="F9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" t="s">
+        <v>208</v>
+      </c>
+      <c r="L9" t="s">
+        <v>209</v>
+      </c>
+      <c r="N9" t="s">
         <v>210</v>
       </c>
-      <c r="G9" t="s">
+      <c r="O9" t="s">
         <v>211</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" t="s">
         <v>212</v>
       </c>
-      <c r="N9" t="s">
+      <c r="Q9" t="s">
         <v>213</v>
       </c>
-      <c r="O9" t="s">
+      <c r="T9" t="s">
         <v>214</v>
       </c>
-      <c r="P9" t="s">
+      <c r="U9" t="s">
         <v>215</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="V9" t="s">
         <v>216</v>
       </c>
-      <c r="T9" t="s">
+      <c r="W9" t="s">
         <v>217</v>
       </c>
-      <c r="U9" t="s">
+      <c r="Y9" t="s">
         <v>218</v>
-      </c>
-      <c r="V9" t="s">
-        <v>219</v>
-      </c>
-      <c r="W9" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -3264,40 +3263,40 @@
         <v>2011</v>
       </c>
       <c r="F10" t="s">
+        <v>219</v>
+      </c>
+      <c r="G10" t="s">
+        <v>220</v>
+      </c>
+      <c r="L10" t="s">
+        <v>221</v>
+      </c>
+      <c r="N10" t="s">
         <v>222</v>
       </c>
-      <c r="G10" t="s">
+      <c r="O10" t="s">
         <v>223</v>
       </c>
-      <c r="L10" t="s">
+      <c r="P10" t="s">
         <v>224</v>
       </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
+        <v>115</v>
+      </c>
+      <c r="T10" t="s">
         <v>225</v>
       </c>
-      <c r="O10" t="s">
+      <c r="U10" t="s">
         <v>226</v>
       </c>
-      <c r="P10" t="s">
+      <c r="V10" t="s">
         <v>227</v>
       </c>
-      <c r="Q10" t="s">
-        <v>118</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="W10" t="s">
         <v>228</v>
       </c>
-      <c r="U10" t="s">
+      <c r="Y10" t="s">
         <v>229</v>
-      </c>
-      <c r="V10" t="s">
-        <v>230</v>
-      </c>
-      <c r="W10" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -3311,40 +3310,40 @@
         <v>2010</v>
       </c>
       <c r="F11" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L11" t="s">
+        <v>232</v>
+      </c>
+      <c r="N11" t="s">
         <v>233</v>
       </c>
-      <c r="G11" t="s">
+      <c r="O11" t="s">
         <v>234</v>
       </c>
-      <c r="L11" t="s">
+      <c r="P11" t="s">
         <v>235</v>
       </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
         <v>236</v>
       </c>
-      <c r="O11" t="s">
+      <c r="T11" t="s">
         <v>237</v>
       </c>
-      <c r="P11" t="s">
+      <c r="U11" t="s">
         <v>238</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="V11" t="s">
         <v>239</v>
       </c>
-      <c r="T11" t="s">
+      <c r="W11" t="s">
         <v>240</v>
       </c>
-      <c r="U11" t="s">
+      <c r="Y11" t="s">
         <v>241</v>
-      </c>
-      <c r="V11" t="s">
-        <v>242</v>
-      </c>
-      <c r="W11" t="s">
-        <v>243</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -3358,40 +3357,40 @@
         <v>2009</v>
       </c>
       <c r="F12" t="s">
+        <v>242</v>
+      </c>
+      <c r="G12" t="s">
+        <v>243</v>
+      </c>
+      <c r="L12" t="s">
+        <v>244</v>
+      </c>
+      <c r="N12" t="s">
         <v>245</v>
       </c>
-      <c r="G12" t="s">
+      <c r="O12" t="s">
         <v>246</v>
       </c>
-      <c r="L12" t="s">
+      <c r="P12" t="s">
         <v>247</v>
       </c>
-      <c r="N12" t="s">
+      <c r="Q12" t="s">
         <v>248</v>
       </c>
-      <c r="O12" t="s">
+      <c r="T12" t="s">
         <v>249</v>
       </c>
-      <c r="P12" t="s">
+      <c r="U12" t="s">
         <v>250</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="V12" t="s">
         <v>251</v>
       </c>
-      <c r="T12" t="s">
+      <c r="W12" t="s">
         <v>252</v>
       </c>
-      <c r="U12" t="s">
+      <c r="Y12" t="s">
         <v>253</v>
-      </c>
-      <c r="V12" t="s">
-        <v>254</v>
-      </c>
-      <c r="W12" t="s">
-        <v>255</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -3402,34 +3401,34 @@
         <v>2008</v>
       </c>
       <c r="F13" t="s">
+        <v>254</v>
+      </c>
+      <c r="G13" t="s">
+        <v>255</v>
+      </c>
+      <c r="L13" t="s">
+        <v>256</v>
+      </c>
+      <c r="N13" t="s">
         <v>257</v>
       </c>
-      <c r="G13" t="s">
+      <c r="O13" t="s">
         <v>258</v>
       </c>
-      <c r="L13" t="s">
+      <c r="P13" t="s">
         <v>259</v>
       </c>
-      <c r="N13" t="s">
+      <c r="Q13" t="s">
         <v>260</v>
       </c>
-      <c r="O13" t="s">
+      <c r="T13" t="s">
         <v>261</v>
       </c>
-      <c r="P13" t="s">
+      <c r="W13" t="s">
         <v>262</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Y13" t="s">
         <v>263</v>
-      </c>
-      <c r="T13" t="s">
-        <v>264</v>
-      </c>
-      <c r="W13" t="s">
-        <v>265</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -3440,31 +3439,31 @@
         <v>2007</v>
       </c>
       <c r="F14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" t="s">
+        <v>265</v>
+      </c>
+      <c r="L14" t="s">
+        <v>266</v>
+      </c>
+      <c r="N14" t="s">
         <v>267</v>
       </c>
-      <c r="G14" t="s">
+      <c r="P14" t="s">
         <v>268</v>
       </c>
-      <c r="L14" t="s">
+      <c r="Q14" t="s">
         <v>269</v>
       </c>
-      <c r="N14" t="s">
+      <c r="T14" t="s">
         <v>270</v>
       </c>
-      <c r="P14" t="s">
+      <c r="W14" t="s">
         <v>271</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Y14" t="s">
         <v>272</v>
-      </c>
-      <c r="T14" t="s">
-        <v>273</v>
-      </c>
-      <c r="W14" t="s">
-        <v>274</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -3475,31 +3474,31 @@
         <v>2006</v>
       </c>
       <c r="F15" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15" t="s">
+        <v>274</v>
+      </c>
+      <c r="L15" t="s">
+        <v>275</v>
+      </c>
+      <c r="N15" t="s">
         <v>276</v>
       </c>
-      <c r="G15" t="s">
+      <c r="P15" t="s">
         <v>277</v>
       </c>
-      <c r="L15" t="s">
+      <c r="Q15" t="s">
         <v>278</v>
       </c>
-      <c r="N15" t="s">
+      <c r="T15" t="s">
         <v>279</v>
       </c>
-      <c r="P15" t="s">
+      <c r="W15" t="s">
         <v>280</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Y15" t="s">
         <v>281</v>
-      </c>
-      <c r="T15" t="s">
-        <v>282</v>
-      </c>
-      <c r="W15" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -3510,31 +3509,31 @@
         <v>2005</v>
       </c>
       <c r="F16" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G16" t="s">
+        <v>282</v>
+      </c>
+      <c r="L16" t="s">
+        <v>283</v>
+      </c>
+      <c r="N16" t="s">
+        <v>284</v>
+      </c>
+      <c r="P16" t="s">
         <v>285</v>
       </c>
-      <c r="L16" t="s">
+      <c r="Q16" t="s">
         <v>286</v>
       </c>
-      <c r="N16" t="s">
+      <c r="T16" t="s">
         <v>287</v>
       </c>
-      <c r="P16" t="s">
+      <c r="W16" t="s">
         <v>288</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Y16" t="s">
         <v>289</v>
-      </c>
-      <c r="T16" t="s">
-        <v>290</v>
-      </c>
-      <c r="W16" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="17" spans="3:23" x14ac:dyDescent="0.25">
@@ -3545,28 +3544,28 @@
         <v>2004</v>
       </c>
       <c r="F17" t="s">
+        <v>290</v>
+      </c>
+      <c r="G17" t="s">
+        <v>291</v>
+      </c>
+      <c r="L17" t="s">
+        <v>292</v>
+      </c>
+      <c r="N17" t="s">
         <v>293</v>
       </c>
-      <c r="G17" t="s">
+      <c r="P17" t="s">
         <v>294</v>
       </c>
-      <c r="L17" t="s">
+      <c r="Q17" t="s">
         <v>295</v>
       </c>
-      <c r="N17" t="s">
+      <c r="T17" t="s">
         <v>296</v>
       </c>
-      <c r="P17" t="s">
+      <c r="W17" t="s">
         <v>297</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>298</v>
-      </c>
-      <c r="T17" t="s">
-        <v>299</v>
-      </c>
-      <c r="W17" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="18" spans="3:23" x14ac:dyDescent="0.25">
@@ -3577,28 +3576,28 @@
         <v>2003</v>
       </c>
       <c r="F18" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" t="s">
+        <v>299</v>
+      </c>
+      <c r="L18" t="s">
+        <v>300</v>
+      </c>
+      <c r="N18" t="s">
         <v>301</v>
       </c>
-      <c r="G18" t="s">
+      <c r="P18" t="s">
         <v>302</v>
       </c>
-      <c r="L18" t="s">
+      <c r="Q18" t="s">
+        <v>246</v>
+      </c>
+      <c r="T18" t="s">
         <v>303</v>
       </c>
-      <c r="N18" t="s">
+      <c r="W18" t="s">
         <v>304</v>
-      </c>
-      <c r="P18" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>249</v>
-      </c>
-      <c r="T18" t="s">
-        <v>306</v>
-      </c>
-      <c r="W18" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="19" spans="3:23" x14ac:dyDescent="0.25">
@@ -3609,28 +3608,28 @@
         <v>2002</v>
       </c>
       <c r="F19" t="s">
+        <v>305</v>
+      </c>
+      <c r="G19" t="s">
+        <v>306</v>
+      </c>
+      <c r="L19" t="s">
+        <v>307</v>
+      </c>
+      <c r="N19" t="s">
         <v>308</v>
       </c>
-      <c r="G19" t="s">
+      <c r="P19" t="s">
         <v>309</v>
       </c>
-      <c r="L19" t="s">
+      <c r="Q19" t="s">
         <v>310</v>
       </c>
-      <c r="N19" t="s">
+      <c r="T19" t="s">
         <v>311</v>
       </c>
-      <c r="P19" t="s">
+      <c r="W19" t="s">
         <v>312</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>313</v>
-      </c>
-      <c r="T19" t="s">
-        <v>314</v>
-      </c>
-      <c r="W19" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="20" spans="3:23" x14ac:dyDescent="0.25">
@@ -3641,25 +3640,25 @@
         <v>2001</v>
       </c>
       <c r="F20" t="s">
+        <v>313</v>
+      </c>
+      <c r="G20" t="s">
+        <v>314</v>
+      </c>
+      <c r="L20" t="s">
+        <v>315</v>
+      </c>
+      <c r="N20" t="s">
         <v>316</v>
       </c>
-      <c r="G20" t="s">
+      <c r="P20" t="s">
         <v>317</v>
       </c>
-      <c r="L20" t="s">
+      <c r="Q20" t="s">
         <v>318</v>
       </c>
-      <c r="N20" t="s">
+      <c r="T20" t="s">
         <v>319</v>
-      </c>
-      <c r="P20" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>321</v>
-      </c>
-      <c r="T20" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="21" spans="3:23" x14ac:dyDescent="0.25">
@@ -3670,25 +3669,25 @@
         <v>2000</v>
       </c>
       <c r="F21" t="s">
+        <v>320</v>
+      </c>
+      <c r="G21" t="s">
+        <v>321</v>
+      </c>
+      <c r="L21" t="s">
+        <v>322</v>
+      </c>
+      <c r="N21" t="s">
         <v>323</v>
       </c>
-      <c r="G21" t="s">
+      <c r="P21" t="s">
         <v>324</v>
       </c>
-      <c r="L21" t="s">
+      <c r="Q21" t="s">
         <v>325</v>
       </c>
-      <c r="N21" t="s">
+      <c r="T21" t="s">
         <v>326</v>
-      </c>
-      <c r="P21" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>328</v>
-      </c>
-      <c r="T21" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="22" spans="3:23" x14ac:dyDescent="0.25">
@@ -3699,19 +3698,19 @@
         <v>1999</v>
       </c>
       <c r="F22" t="s">
+        <v>327</v>
+      </c>
+      <c r="G22" t="s">
+        <v>328</v>
+      </c>
+      <c r="L22" t="s">
+        <v>329</v>
+      </c>
+      <c r="P22" t="s">
         <v>330</v>
       </c>
-      <c r="G22" t="s">
+      <c r="T22" t="s">
         <v>331</v>
-      </c>
-      <c r="L22" t="s">
-        <v>332</v>
-      </c>
-      <c r="P22" t="s">
-        <v>333</v>
-      </c>
-      <c r="T22" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.25">
@@ -3722,19 +3721,19 @@
         <v>1998</v>
       </c>
       <c r="F23" t="s">
+        <v>332</v>
+      </c>
+      <c r="G23" t="s">
+        <v>333</v>
+      </c>
+      <c r="L23" t="s">
+        <v>334</v>
+      </c>
+      <c r="P23" t="s">
         <v>335</v>
       </c>
-      <c r="G23" t="s">
+      <c r="T23" t="s">
         <v>336</v>
-      </c>
-      <c r="L23" t="s">
-        <v>337</v>
-      </c>
-      <c r="P23" t="s">
-        <v>338</v>
-      </c>
-      <c r="T23" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="24" spans="3:23" x14ac:dyDescent="0.25">
@@ -3745,19 +3744,19 @@
         <v>1997</v>
       </c>
       <c r="F24" t="s">
+        <v>337</v>
+      </c>
+      <c r="G24" t="s">
+        <v>338</v>
+      </c>
+      <c r="L24" t="s">
+        <v>339</v>
+      </c>
+      <c r="P24" t="s">
         <v>340</v>
       </c>
-      <c r="G24" t="s">
+      <c r="T24" t="s">
         <v>341</v>
-      </c>
-      <c r="L24" t="s">
-        <v>342</v>
-      </c>
-      <c r="P24" t="s">
-        <v>343</v>
-      </c>
-      <c r="T24" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="25" spans="3:23" x14ac:dyDescent="0.25">
@@ -3768,19 +3767,19 @@
         <v>1996</v>
       </c>
       <c r="F25" t="s">
+        <v>342</v>
+      </c>
+      <c r="G25" t="s">
+        <v>343</v>
+      </c>
+      <c r="L25" t="s">
+        <v>344</v>
+      </c>
+      <c r="P25" t="s">
         <v>345</v>
       </c>
-      <c r="G25" t="s">
+      <c r="T25" t="s">
         <v>346</v>
-      </c>
-      <c r="L25" t="s">
-        <v>347</v>
-      </c>
-      <c r="P25" t="s">
-        <v>348</v>
-      </c>
-      <c r="T25" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="26" spans="3:23" x14ac:dyDescent="0.25">
@@ -3791,19 +3790,19 @@
         <v>1995</v>
       </c>
       <c r="F26" t="s">
+        <v>347</v>
+      </c>
+      <c r="G26" t="s">
+        <v>348</v>
+      </c>
+      <c r="L26" t="s">
+        <v>349</v>
+      </c>
+      <c r="P26" t="s">
         <v>350</v>
       </c>
-      <c r="G26" t="s">
+      <c r="T26" t="s">
         <v>351</v>
-      </c>
-      <c r="L26" t="s">
-        <v>352</v>
-      </c>
-      <c r="P26" t="s">
-        <v>353</v>
-      </c>
-      <c r="T26" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="27" spans="3:23" x14ac:dyDescent="0.25">
@@ -3814,19 +3813,19 @@
         <v>1994</v>
       </c>
       <c r="F27" t="s">
+        <v>352</v>
+      </c>
+      <c r="G27" t="s">
+        <v>353</v>
+      </c>
+      <c r="L27" t="s">
+        <v>354</v>
+      </c>
+      <c r="P27" t="s">
         <v>355</v>
       </c>
-      <c r="G27" t="s">
+      <c r="T27" t="s">
         <v>356</v>
-      </c>
-      <c r="L27" t="s">
-        <v>357</v>
-      </c>
-      <c r="P27" t="s">
-        <v>358</v>
-      </c>
-      <c r="T27" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.25">
@@ -3837,19 +3836,19 @@
         <v>1993</v>
       </c>
       <c r="F28" t="s">
+        <v>357</v>
+      </c>
+      <c r="G28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L28" t="s">
+        <v>359</v>
+      </c>
+      <c r="P28" t="s">
         <v>360</v>
       </c>
-      <c r="G28" t="s">
+      <c r="T28" t="s">
         <v>361</v>
-      </c>
-      <c r="L28" t="s">
-        <v>362</v>
-      </c>
-      <c r="P28" t="s">
-        <v>363</v>
-      </c>
-      <c r="T28" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="29" spans="3:23" x14ac:dyDescent="0.25">
@@ -3860,19 +3859,19 @@
         <v>1992</v>
       </c>
       <c r="F29" t="s">
+        <v>362</v>
+      </c>
+      <c r="G29" t="s">
+        <v>363</v>
+      </c>
+      <c r="L29" t="s">
+        <v>364</v>
+      </c>
+      <c r="P29" t="s">
         <v>365</v>
       </c>
-      <c r="G29" t="s">
+      <c r="T29" t="s">
         <v>366</v>
-      </c>
-      <c r="L29" t="s">
-        <v>367</v>
-      </c>
-      <c r="P29" t="s">
-        <v>368</v>
-      </c>
-      <c r="T29" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="30" spans="3:23" x14ac:dyDescent="0.25">
@@ -3883,19 +3882,19 @@
         <v>1991</v>
       </c>
       <c r="F30" t="s">
+        <v>367</v>
+      </c>
+      <c r="G30" t="s">
+        <v>368</v>
+      </c>
+      <c r="L30" t="s">
+        <v>369</v>
+      </c>
+      <c r="P30" t="s">
         <v>370</v>
       </c>
-      <c r="G30" t="s">
+      <c r="T30" t="s">
         <v>371</v>
-      </c>
-      <c r="L30" t="s">
-        <v>372</v>
-      </c>
-      <c r="P30" t="s">
-        <v>373</v>
-      </c>
-      <c r="T30" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="31" spans="3:23" x14ac:dyDescent="0.25">
@@ -3906,16 +3905,16 @@
         <v>1990</v>
       </c>
       <c r="F31" t="s">
+        <v>372</v>
+      </c>
+      <c r="G31" t="s">
+        <v>373</v>
+      </c>
+      <c r="L31" t="s">
+        <v>374</v>
+      </c>
+      <c r="T31" t="s">
         <v>375</v>
-      </c>
-      <c r="G31" t="s">
-        <v>376</v>
-      </c>
-      <c r="L31" t="s">
-        <v>377</v>
-      </c>
-      <c r="T31" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="32" spans="3:23" x14ac:dyDescent="0.25">
@@ -3923,16 +3922,16 @@
         <v>1989</v>
       </c>
       <c r="F32" t="s">
+        <v>376</v>
+      </c>
+      <c r="G32" t="s">
+        <v>377</v>
+      </c>
+      <c r="L32" t="s">
+        <v>378</v>
+      </c>
+      <c r="T32" t="s">
         <v>379</v>
-      </c>
-      <c r="G32" t="s">
-        <v>380</v>
-      </c>
-      <c r="L32" t="s">
-        <v>381</v>
-      </c>
-      <c r="T32" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="33" spans="5:20" x14ac:dyDescent="0.25">
@@ -3940,16 +3939,16 @@
         <v>1988</v>
       </c>
       <c r="F33" t="s">
+        <v>380</v>
+      </c>
+      <c r="G33" t="s">
+        <v>381</v>
+      </c>
+      <c r="L33" t="s">
+        <v>382</v>
+      </c>
+      <c r="T33" t="s">
         <v>383</v>
-      </c>
-      <c r="G33" t="s">
-        <v>384</v>
-      </c>
-      <c r="L33" t="s">
-        <v>385</v>
-      </c>
-      <c r="T33" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="34" spans="5:20" x14ac:dyDescent="0.25">
@@ -3957,16 +3956,16 @@
         <v>1987</v>
       </c>
       <c r="F34" t="s">
+        <v>384</v>
+      </c>
+      <c r="G34" t="s">
+        <v>385</v>
+      </c>
+      <c r="L34" t="s">
+        <v>386</v>
+      </c>
+      <c r="T34" t="s">
         <v>387</v>
-      </c>
-      <c r="G34" t="s">
-        <v>388</v>
-      </c>
-      <c r="L34" t="s">
-        <v>389</v>
-      </c>
-      <c r="T34" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="35" spans="5:20" x14ac:dyDescent="0.25">
@@ -3974,16 +3973,16 @@
         <v>1986</v>
       </c>
       <c r="F35" t="s">
+        <v>388</v>
+      </c>
+      <c r="G35" t="s">
+        <v>389</v>
+      </c>
+      <c r="L35" t="s">
+        <v>390</v>
+      </c>
+      <c r="T35" t="s">
         <v>391</v>
-      </c>
-      <c r="G35" t="s">
-        <v>392</v>
-      </c>
-      <c r="L35" t="s">
-        <v>393</v>
-      </c>
-      <c r="T35" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="36" spans="5:20" x14ac:dyDescent="0.25">
@@ -3991,16 +3990,16 @@
         <v>1985</v>
       </c>
       <c r="F36" t="s">
+        <v>392</v>
+      </c>
+      <c r="G36" t="s">
+        <v>393</v>
+      </c>
+      <c r="L36" t="s">
+        <v>394</v>
+      </c>
+      <c r="T36" t="s">
         <v>395</v>
-      </c>
-      <c r="G36" t="s">
-        <v>396</v>
-      </c>
-      <c r="L36" t="s">
-        <v>397</v>
-      </c>
-      <c r="T36" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="37" spans="5:20" x14ac:dyDescent="0.25">
@@ -4008,13 +4007,13 @@
         <v>1984</v>
       </c>
       <c r="F37" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G37" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="T37" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" spans="5:20" x14ac:dyDescent="0.25">
@@ -4022,13 +4021,13 @@
         <v>1983</v>
       </c>
       <c r="F38" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G38" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="T38" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="5:20" x14ac:dyDescent="0.25">
@@ -4036,13 +4035,13 @@
         <v>1982</v>
       </c>
       <c r="F39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G39" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T39" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" spans="5:20" x14ac:dyDescent="0.25">
@@ -4050,13 +4049,13 @@
         <v>1981</v>
       </c>
       <c r="F40" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G40" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="T40" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="5:20" x14ac:dyDescent="0.25">
@@ -4064,13 +4063,13 @@
         <v>1980</v>
       </c>
       <c r="F41" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G41" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="T41" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="5:20" x14ac:dyDescent="0.25">
@@ -4078,13 +4077,13 @@
         <v>1979</v>
       </c>
       <c r="F42" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G42" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="T42" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="43" spans="5:20" x14ac:dyDescent="0.25">
@@ -4092,13 +4091,13 @@
         <v>1978</v>
       </c>
       <c r="F43" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G43" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="T43" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="44" spans="5:20" x14ac:dyDescent="0.25">
@@ -4106,13 +4105,13 @@
         <v>1977</v>
       </c>
       <c r="F44" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G44" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="T44" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="45" spans="5:20" x14ac:dyDescent="0.25">
@@ -4120,13 +4119,13 @@
         <v>1976</v>
       </c>
       <c r="F45" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G45" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="T45" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="46" spans="5:20" x14ac:dyDescent="0.25">
@@ -4134,13 +4133,13 @@
         <v>1975</v>
       </c>
       <c r="F46" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G46" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="T46" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="5:20" x14ac:dyDescent="0.25">
@@ -4148,10 +4147,10 @@
         <v>1974</v>
       </c>
       <c r="F47" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="T47" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="48" spans="5:20" x14ac:dyDescent="0.25">
@@ -4159,10 +4158,10 @@
         <v>1973</v>
       </c>
       <c r="F48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="T48" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="49" spans="5:20" x14ac:dyDescent="0.25">
@@ -4170,10 +4169,10 @@
         <v>1972</v>
       </c>
       <c r="F49" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="T49" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="50" spans="5:20" x14ac:dyDescent="0.25">
@@ -4181,586 +4180,586 @@
         <v>1971</v>
       </c>
       <c r="F50" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="T50" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="51" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="T51" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="T52" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="53" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="T53" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="T54" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="T55" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="T56" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="T57" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="T58" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="59" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="T59" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="60" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="T60" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="61" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="T61" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="62" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="T62" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="63" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="T63" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" spans="5:20" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="T64" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="65" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="T65" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="T66" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="T67" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="T68" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="69" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="T69" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="70" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="T70" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="71" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="T71" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="72" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="T72" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="73" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="T73" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="74" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="T74" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="75" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="T75" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="76" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="T76" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="77" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="T77" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="78" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="T78" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="79" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="T79" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="80" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="T80" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="81" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="T81" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="82" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="T82" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="83" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="T83" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="84" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T84" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T85" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="86" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="T86" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="87" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="T87" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="88" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T88" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T89" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="90" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T90" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="91" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T91" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="92" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T92" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="93" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T93" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="94" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T94" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="95" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T95" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="96" spans="6:20" x14ac:dyDescent="0.25">
       <c r="T96" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="97" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T97" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="98" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T98" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T99" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="100" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T100" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="101" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T101" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="102" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T102" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="103" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T103" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="104" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T104" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="105" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T105" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="106" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T106" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="107" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T107" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T108" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="109" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T109" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="110" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T110" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="111" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T111" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="112" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T112" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="113" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T113" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="114" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T114" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="115" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T115" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="116" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T116" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="117" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T117" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="118" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T118" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="119" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T119" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="120" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T120" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="121" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T121" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T122" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="123" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T123" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="124" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T124" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="125" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T125" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="126" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T126" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="127" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T127" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="128" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T128" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="129" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T129" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="130" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T130" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="131" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T131" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="132" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T132" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="133" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T133" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="134" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T134" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="135" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T135" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="136" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T136" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="137" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T137" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="138" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T138" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="139" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T139" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T140" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="141" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T141" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="142" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T142" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="143" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T143" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>